<commit_message>
edit all lan 2
</commit_message>
<xml_diff>
--- a/templates/sample-info.xlsx
+++ b/templates/sample-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0985A1-EB8F-4AB3-8168-E5F20D8E15BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71643A2-12E5-4251-9AD5-92D35B00B3FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="17" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -73,36 +73,33 @@
     <t>Phòng Hành chính</t>
   </si>
   <si>
+    <t>Mã cấp trên</t>
+  </si>
+  <si>
+    <t>Tên viết tắt</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Mô tả phòng hành chính</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
     <t>Phòng Dịch vụ</t>
   </si>
   <si>
-    <t>Mã cấp trên</t>
-  </si>
-  <si>
-    <t>Tên viết tắt</t>
-  </si>
-  <si>
-    <t>Mô tả</t>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>Mô tả phòng dịch vụ</t>
   </si>
   <si>
     <t>Phòng Tự động</t>
   </si>
   <si>
-    <t>HC</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>TĐ</t>
-  </si>
-  <si>
-    <t>Mô tả phòng hành chính</t>
-  </si>
-  <si>
-    <t>Mô tả phòng dịch vụ</t>
-  </si>
-  <si>
     <t>Mô tả phòng tự động</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Mô tả giải lao</t>
+  </si>
+  <si>
+    <t>TD</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -744,16 +744,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -763,16 +763,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -783,16 +780,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -803,16 +797,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -823,16 +814,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>1</v>

</xml_diff>